<commit_message>
Chiapas, Chihuahua, Ciudad de México, Estado de México, Querétaro
</commit_message>
<xml_diff>
--- a/Resources/data/Versión_2.0/Compilado de Entidades Federativas 2.0.xlsx
+++ b/Resources/data/Versión_2.0/Compilado de Entidades Federativas 2.0.xlsx
@@ -1750,9 +1750,9 @@
   <dimension ref="A3:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>

</xml_diff>